<commit_message>
explain how the api algorithm will work
</commit_message>
<xml_diff>
--- a/ride_assignments.xlsx
+++ b/ride_assignments.xlsx
@@ -605,52 +605,52 @@
       </c>
       <c r="D3" s="7" t="inlineStr">
         <is>
-          <t>Elie Park</t>
-        </is>
-      </c>
-      <c r="E3" s="7" t="inlineStr">
+          <t>Aaron duong</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Ethan Yu</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="G3" s="6" t="inlineStr">
+        <is>
+          <t>Gabriel Ni</t>
+        </is>
+      </c>
+      <c r="J3" s="8" t="inlineStr">
+        <is>
+          <t>Flexible 💚</t>
+        </is>
+      </c>
+      <c r="K3" s="7" t="inlineStr">
+        <is>
+          <t>Jiwang Lee</t>
+        </is>
+      </c>
+      <c r="L3" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">derek liang </t>
+        </is>
+      </c>
+      <c r="M3" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Darius Ajebon </t>
+        </is>
+      </c>
+      <c r="N3" s="1" t="inlineStr">
+        <is>
+          <t>Christina Ko</t>
+        </is>
+      </c>
+      <c r="O3" s="7" t="inlineStr">
         <is>
           <t>Hannah Kim</t>
-        </is>
-      </c>
-      <c r="F3" s="7" t="inlineStr">
-        <is>
-          <t>Ella Lu</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>Emily Yang</t>
-        </is>
-      </c>
-      <c r="J3" s="8" t="inlineStr">
-        <is>
-          <t>Flexible 💚</t>
-        </is>
-      </c>
-      <c r="K3" s="7" t="inlineStr">
-        <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
-      <c r="L3" s="1" t="inlineStr">
-        <is>
-          <t>Grace Park</t>
-        </is>
-      </c>
-      <c r="M3" s="7" t="inlineStr">
-        <is>
-          <t>Rachel Kim</t>
-        </is>
-      </c>
-      <c r="N3" s="6" t="inlineStr">
-        <is>
-          <t>Daniel Song</t>
-        </is>
-      </c>
-      <c r="O3" s="7" t="inlineStr">
-        <is>
-          <t>Taeho Choe</t>
         </is>
       </c>
     </row>
@@ -667,22 +667,22 @@
       </c>
       <c r="D4" s="7" t="inlineStr">
         <is>
-          <t>Hannah Zhang</t>
-        </is>
-      </c>
-      <c r="E4" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">derek liang </t>
+          <t>Ella Lu</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Joanna Wei</t>
         </is>
       </c>
       <c r="F4" s="7" t="inlineStr">
         <is>
-          <t>Ella</t>
+          <t>Israel Haile</t>
         </is>
       </c>
       <c r="G4" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Daniel Kim </t>
+          <t>Lucy Han</t>
         </is>
       </c>
       <c r="J4" s="10" t="inlineStr">
@@ -692,27 +692,27 @@
       </c>
       <c r="K4" s="7" t="inlineStr">
         <is>
-          <t>Hannah Kim</t>
-        </is>
-      </c>
-      <c r="L4" s="1" t="inlineStr">
+          <t>Israel Haile</t>
+        </is>
+      </c>
+      <c r="L4" s="7" t="inlineStr">
+        <is>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="M4" s="6" t="inlineStr">
+        <is>
+          <t>Lucy Han</t>
+        </is>
+      </c>
+      <c r="N4" s="1" t="inlineStr">
         <is>
           <t>Sehyun Jung</t>
         </is>
       </c>
-      <c r="M4" s="7" t="inlineStr">
-        <is>
-          <t>Daniel Kuo</t>
-        </is>
-      </c>
-      <c r="N4" s="6" t="inlineStr">
-        <is>
-          <t>Emily Yang</t>
-        </is>
-      </c>
       <c r="O4" s="7" t="inlineStr">
         <is>
-          <t>Aaron duong</t>
+          <t>Kyle Hwang</t>
         </is>
       </c>
     </row>
@@ -724,17 +724,17 @@
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>Nathanael Wang</t>
+          <t>Grace Park</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>Aaron duong</t>
-        </is>
-      </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>Hyeongjun Son</t>
+          <t xml:space="preserve">Maya Habraken </t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>Sehyun Jung</t>
         </is>
       </c>
       <c r="F5" s="7" t="inlineStr">
@@ -744,7 +744,7 @@
       </c>
       <c r="G5" s="6" t="inlineStr">
         <is>
-          <t>Gabriel Ni</t>
+          <t xml:space="preserve">Daniel Kim </t>
         </is>
       </c>
       <c r="J5" s="11" t="inlineStr">
@@ -754,69 +754,69 @@
       </c>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grace Sowon Park </t>
-        </is>
-      </c>
-      <c r="L5" s="1" t="inlineStr">
-        <is>
-          <t>Christina Ko</t>
-        </is>
-      </c>
-      <c r="M5" s="7" t="inlineStr">
-        <is>
-          <t>Kyle Hwang</t>
-        </is>
-      </c>
-      <c r="N5" s="6" t="inlineStr">
-        <is>
-          <t>Lucy Han</t>
+          <t>Rachel Kim</t>
+        </is>
+      </c>
+      <c r="L5" s="7" t="inlineStr">
+        <is>
+          <t>Taeho Choe</t>
+        </is>
+      </c>
+      <c r="M5" s="6" t="inlineStr">
+        <is>
+          <t>Emily Yang</t>
+        </is>
+      </c>
+      <c r="N5" s="1" t="inlineStr">
+        <is>
+          <t>Grace Park</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>Grace Park</t>
+          <t>Nathanael Wang</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>Jiwang Lee</t>
-        </is>
-      </c>
-      <c r="E6" s="7" t="inlineStr">
-        <is>
-          <t>Kyle Hwang</t>
+          <t>Grace Kwon</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>JJ Lee</t>
         </is>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t>Jeffery Huang</t>
+          <t>Taeho Choe</t>
         </is>
       </c>
       <c r="G6" s="6" t="inlineStr">
         <is>
-          <t>helena song</t>
+          <t>Daniel Song</t>
         </is>
       </c>
       <c r="K6" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">derek liang </t>
-        </is>
-      </c>
-      <c r="L6" s="1" t="inlineStr">
+          <t>Aaron duong</t>
+        </is>
+      </c>
+      <c r="L6" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grace Sowon Park </t>
+        </is>
+      </c>
+      <c r="M6" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Daniel Kim </t>
+        </is>
+      </c>
+      <c r="N6" s="1" t="inlineStr">
         <is>
           <t>Nathanael Wang</t>
-        </is>
-      </c>
-      <c r="M6" s="7" t="inlineStr">
-        <is>
-          <t>Israel Haile</t>
-        </is>
-      </c>
-      <c r="N6" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Darius Ajebon </t>
         </is>
       </c>
     </row>
@@ -895,16 +895,16 @@
           <t>Pedro Flores-Teran</t>
         </is>
       </c>
-      <c r="K10" s="7" t="inlineStr">
-        <is>
-          <t>Ella Lu</t>
-        </is>
-      </c>
-      <c r="L10" s="9" t="inlineStr">
+      <c r="K10" s="9" t="inlineStr">
         <is>
           <t>April Tong</t>
         </is>
       </c>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>Joann Jung</t>
+        </is>
+      </c>
       <c r="M10" s="6" t="inlineStr">
         <is>
           <t>Gabriel Ni</t>
@@ -917,7 +917,7 @@
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
+          <t>Grace Kwon</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t>김예림</t>
+          <t>Faith Chen</t>
         </is>
       </c>
       <c r="G11" s="9" t="inlineStr">
@@ -937,16 +937,16 @@
           <t>Shayla Nguyen</t>
         </is>
       </c>
-      <c r="K11" s="7" t="inlineStr">
+      <c r="K11" s="9" t="inlineStr">
+        <is>
+          <t>Pedro Flores-Teran</t>
+        </is>
+      </c>
+      <c r="L11" s="7" t="inlineStr">
         <is>
           <t>Hyeongjun Son</t>
         </is>
       </c>
-      <c r="L11" s="9" t="inlineStr">
-        <is>
-          <t>Sam Ko</t>
-        </is>
-      </c>
       <c r="M11" s="6" t="inlineStr">
         <is>
           <t>Jocelyn Youn</t>
@@ -954,7 +954,7 @@
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
-          <t>Hannah Zhang</t>
+          <t>Benjamin Kim</t>
         </is>
       </c>
     </row>
@@ -966,17 +966,17 @@
       </c>
       <c r="G12" s="9" t="inlineStr">
         <is>
-          <t>Faith Chen</t>
-        </is>
-      </c>
-      <c r="K12" s="7" t="inlineStr">
-        <is>
-          <t>Joann Jung</t>
-        </is>
-      </c>
-      <c r="L12" s="9" t="inlineStr">
-        <is>
-          <t>Pedro Flores-Teran</t>
+          <t>Austin Lee</t>
+        </is>
+      </c>
+      <c r="K12" s="9" t="inlineStr">
+        <is>
+          <t>Shayla Nguyen</t>
+        </is>
+      </c>
+      <c r="L12" s="7" t="inlineStr">
+        <is>
+          <t>Ella Lu</t>
         </is>
       </c>
       <c r="M12" s="9" t="inlineStr">
@@ -986,29 +986,29 @@
       </c>
       <c r="O12" s="7" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
+          <t>Hannah Zhang</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="G13" s="9" t="inlineStr">
         <is>
-          <t>Austin Lee</t>
-        </is>
-      </c>
-      <c r="K13" s="7" t="inlineStr">
+          <t>김예림</t>
+        </is>
+      </c>
+      <c r="K13" s="9" t="inlineStr">
+        <is>
+          <t>Sam Ko</t>
+        </is>
+      </c>
+      <c r="L13" s="7" t="inlineStr">
         <is>
           <t>Ella</t>
         </is>
       </c>
-      <c r="L13" s="9" t="inlineStr">
-        <is>
-          <t>Shayla Nguyen</t>
-        </is>
-      </c>
       <c r="O13" s="7" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
+          <t xml:space="preserve">Maya Habraken </t>
         </is>
       </c>
     </row>
@@ -1064,27 +1064,27 @@
     <row r="17">
       <c r="C17" s="7" t="inlineStr">
         <is>
-          <t>Joann Jung</t>
+          <t>Ella</t>
         </is>
       </c>
       <c r="D17" s="6" t="inlineStr">
         <is>
-          <t>Daniel Song</t>
+          <t>Emily Yang</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Grace Sowon Park </t>
-        </is>
-      </c>
-      <c r="F17" s="1" t="inlineStr">
-        <is>
-          <t>Sehyun Jung</t>
+          <t>Hyeongjun Son</t>
+        </is>
+      </c>
+      <c r="F17" s="7" t="inlineStr">
+        <is>
+          <t>Elie Park</t>
         </is>
       </c>
       <c r="K17" s="1" t="inlineStr">
         <is>
-          <t>JJ Lee</t>
+          <t>Ethan Yu</t>
         </is>
       </c>
       <c r="L17" s="9" t="inlineStr">
@@ -1102,63 +1102,63 @@
           <t>Melody Hong</t>
         </is>
       </c>
-      <c r="P17" s="6" t="inlineStr">
-        <is>
-          <t>Daniel Kim  (Back home 💙)</t>
+      <c r="P17" s="9" t="inlineStr">
+        <is>
+          <t>Jane Yoo (Back home 💙)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="C18" s="7" t="inlineStr">
         <is>
-          <t>Israel Haile</t>
+          <t>Hannah Kim</t>
         </is>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>Lucy Han</t>
+          <t>Jocelyn Youn</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
         <is>
-          <t>Grace Kwon</t>
-        </is>
-      </c>
-      <c r="F18" s="1" t="inlineStr">
-        <is>
-          <t>Ethan Yu</t>
+          <t>Joann Jung</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grace Sowon Park </t>
         </is>
       </c>
       <c r="K18" s="1" t="inlineStr">
         <is>
-          <t>Ethan Yu</t>
-        </is>
-      </c>
-      <c r="P18" s="9" t="inlineStr">
-        <is>
-          <t>Jane Yoo (Back home 💙)</t>
+          <t>JJ Lee</t>
+        </is>
+      </c>
+      <c r="P18" s="6" t="inlineStr">
+        <is>
+          <t>Daniel Song (Back home 💙)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="C19" s="7" t="inlineStr">
         <is>
-          <t>Taeho Choe</t>
+          <t>Jeffery Huang</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>Jocelyn Youn</t>
+          <t>helena song</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>Benjamin Kim</t>
-        </is>
-      </c>
-      <c r="F19" s="1" t="inlineStr">
-        <is>
-          <t>Joanna Wei</t>
+          <t>Daniel Kuo</t>
+        </is>
+      </c>
+      <c r="F19" s="7" t="inlineStr">
+        <is>
+          <t>Kyle Hwang</t>
         </is>
       </c>
       <c r="P19" s="9" t="inlineStr">
@@ -1170,7 +1170,7 @@
     <row r="20">
       <c r="C20" s="7" t="inlineStr">
         <is>
-          <t>Daniel Kuo</t>
+          <t xml:space="preserve">derek liang </t>
         </is>
       </c>
       <c r="D20" s="6" t="inlineStr">
@@ -1180,12 +1180,12 @@
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maya Habraken </t>
-        </is>
-      </c>
-      <c r="F20" s="1" t="inlineStr">
-        <is>
-          <t>JJ Lee</t>
+          <t>Hannah Zhang</t>
+        </is>
+      </c>
+      <c r="F20" s="7" t="inlineStr">
+        <is>
+          <t>Benjamin Kim</t>
         </is>
       </c>
       <c r="P20" s="1" t="inlineStr">

</xml_diff>